<commit_message>
fix(Week02, Week04, Week05): update generated data files and minor formatting fixes
What was changed:
- Updated Week04 example data files (data.csv, data.xlsx, people_with_salary.csv)
- Added Week02 exercise output files (stock_prices, students JSON/CSV)
- Minor formatting updates to Week05 notebooks

Claude Code contributions:
- Committed data files generated from notebook execution
- Updated Week05 notebooks for consistency with Week01-04 fixes
- Ensured all example data files are properly tracked

Manual edits:
- Verified data files are correctly formatted
- Confirmed notebooks execute successfully with new data

🤖 Generated with Claude Code (https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/2025-26/MN5813/Week04/assets/example_data/data.xlsx
+++ b/2025-26/MN5813/Week04/assets/example_data/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -609,7 +609,7 @@
         <v>-0.4694743859349521</v>
       </c>
       <c r="C10" t="n">
-        <v>0.257550390722764</v>
+        <v>0.2575503907227643</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -627,7 +627,7 @@
         <v>0.5425600435859647</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0744459157661671</v>
+        <v>-0.0744459157661672</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.9080240755212112</v>
+        <v>-0.9080240755212108</v>
       </c>
       <c r="C20" t="n">
         <v>1.14282281451502</v>
@@ -1077,7 +1077,7 @@
         <v>0.822544912103189</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.9194242342338034</v>
+        <v>-0.9194242342338032</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>-1.220843649971022</v>
       </c>
       <c r="C37" t="n">
-        <v>1.54993440501754</v>
+        <v>1.549934405017539</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1275,7 +1275,7 @@
         <v>-0.7198442083947086</v>
       </c>
       <c r="C47" t="n">
-        <v>0.78182287177731</v>
+        <v>0.7818228717773104</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1365,7 +1365,7 @@
         <v>0.324083969394795</v>
       </c>
       <c r="C52" t="n">
-        <v>0.2504928503458766</v>
+        <v>0.2504928503458765</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1383,7 +1383,7 @@
         <v>-0.3850822804163165</v>
       </c>
       <c r="C53" t="n">
-        <v>0.3464482094969758</v>
+        <v>0.3464482094969757</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1761,7 +1761,7 @@
         <v>-0.0358260391099515</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.0771017094141041</v>
+        <v>-0.0771017094141042</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1779,7 +1779,7 @@
         <v>1.564643655814006</v>
       </c>
       <c r="C75" t="n">
-        <v>0.3411519748166435</v>
+        <v>0.3411519748166439</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.08704706823817129</v>
+        <v>0.0870470682381712</v>
       </c>
       <c r="C78" t="n">
         <v>0.013001891877907</v>
@@ -1848,7 +1848,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.2990073504658678</v>
+        <v>-0.2990073504658674</v>
       </c>
       <c r="C79" t="n">
         <v>1.453534077157317</v>
@@ -1977,7 +1977,7 @@
         <v>-0.8084936028931876</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.2234627853258508</v>
+        <v>-0.2234627853258509</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -1995,7 +1995,7 @@
         <v>-0.5017570435845365</v>
       </c>
       <c r="C87" t="n">
-        <v>0.7140004940920919</v>
+        <v>0.714000494092092</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2226,7 +2226,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.0051134566424609</v>
+        <v>0.0051134566424608</v>
       </c>
       <c r="C100" t="n">
         <v>0.0582087184459998</v>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-0.2345871333751474</v>
+        <v>-0.2345871333751469</v>
       </c>
       <c r="C101" t="n">
         <v>-1.142970297830623</v>

</xml_diff>